<commit_message>
Parse excel file and produce sql scirript.
</commit_message>
<xml_diff>
--- a/v1/db_scripts/Stomp Master Data.xlsx
+++ b/v1/db_scripts/Stomp Master Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14220" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Brooks</t>
   </si>
@@ -34,12 +34,6 @@
     <t>10:15-11:40</t>
   </si>
   <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Shanon Rose Geary</t>
-  </si>
-  <si>
     <t>brian.bertini@gmail.com</t>
   </si>
   <si>
@@ -49,12 +43,6 @@
     <t>East Somerville</t>
   </si>
   <si>
-    <t>Lisa Fantini</t>
-  </si>
-  <si>
-    <t>Declan Devine</t>
-  </si>
-  <si>
     <t>lisa.fantini@tufts.edu</t>
   </si>
   <si>
@@ -152,6 +140,51 @@
   </si>
   <si>
     <t>"03452"</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Heilbron</t>
+  </si>
+  <si>
+    <t>sheilb01</t>
+  </si>
+  <si>
+    <t>samheilbron@gmail.com</t>
+  </si>
+  <si>
+    <t>UTLN</t>
+  </si>
+  <si>
+    <t>Terrence</t>
+  </si>
+  <si>
+    <t>Roh</t>
+  </si>
+  <si>
+    <t>troh@gmail.com</t>
+  </si>
+  <si>
+    <t>troh01</t>
+  </si>
+  <si>
+    <t>Sam Heilbron</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>george.wright@columbus.edu</t>
+  </si>
+  <si>
+    <t>Terrence Roh</t>
+  </si>
+  <si>
+    <t>10:20-11:45</t>
   </si>
 </sst>
 </file>
@@ -639,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -654,33 +687,33 @@
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1">
       <c r="A1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" s="13">
         <v>6176295440</v>
@@ -688,16 +721,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3" s="13">
         <v>7813932177</v>
@@ -708,13 +741,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E4" s="13">
         <v>6178934545</v>
@@ -732,10 +765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -748,37 +781,53 @@
   <sheetData>
     <row r="1" spans="1:4" s="15" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -789,12 +838,66 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="15" customFormat="1">
+      <c r="A1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -808,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -818,7 +921,7 @@
     <col min="2" max="2" width="9" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.1640625" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32" style="13" bestFit="1" customWidth="1"/>
@@ -826,31 +929,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16">
@@ -866,23 +969,25 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="F2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -890,21 +995,23 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
-        <v>42686</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16">
@@ -1315,6 +1422,10 @@
       <c r="I40" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Fix db init script
</commit_message>
<xml_diff>
--- a/v1/db_scripts/Stomp Master Data.xlsx
+++ b/v1/db_scripts/Stomp Master Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14220" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14220" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>Brooks</t>
   </si>
@@ -233,9 +233,6 @@
     <t>NXT Robotics Kit</t>
   </si>
   <si>
-    <t>Spaghetti Box</t>
-  </si>
-  <si>
     <t>Laptops</t>
   </si>
   <si>
@@ -294,6 +291,12 @@
   </si>
   <si>
     <t>Stomper</t>
+  </si>
+  <si>
+    <t>Spaghetti Boxes</t>
+  </si>
+  <si>
+    <t>Marshmellow Bag</t>
   </si>
 </sst>
 </file>
@@ -982,13 +985,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1039,7 +1042,7 @@
         <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1056,7 +1059,7 @@
         <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1073,41 +1076,41 @@
         <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1241,25 +1244,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="I4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16">
@@ -1675,15 +1678,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" style="13" bestFit="1" customWidth="1"/>
@@ -1743,13 +1746,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="13" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B4" s="13">
         <v>20</v>
       </c>
       <c r="C4" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="13">
         <v>2</v>
@@ -1760,7 +1763,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="13">
         <v>15</v>
@@ -1777,7 +1780,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="13">
         <v>10</v>
@@ -1790,6 +1793,23 @@
       </c>
       <c r="E6" s="13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="13">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>